<commit_message>
Producto falta validacion a update imagen
</commit_message>
<xml_diff>
--- a/docs/Requerimiento.xlsx
+++ b/docs/Requerimiento.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\Apache24\htdocs\viva\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E7F870-3CDD-4E36-B487-202E2083BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9F9256-E7F8-4398-A540-F0BD24E21623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="INDEX_LANDING" sheetId="3" r:id="rId1"/>
+    <sheet name="Landing" sheetId="3" r:id="rId1"/>
     <sheet name="Login " sheetId="7" r:id="rId2"/>
     <sheet name="REGISTRO_VENDEDOR" sheetId="2" r:id="rId3"/>
     <sheet name="MIS_PRODUCTOS" sheetId="4" r:id="rId4"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="303">
   <si>
     <t>SI</t>
   </si>
@@ -304,16 +304,10 @@
     <t>El sistema debe implementar desplazamiento suave al navegar entre secciones.</t>
   </si>
   <si>
-    <t>El sistema debe responder a las interacciones del usuario en menos de 1 segundo.</t>
-  </si>
-  <si>
     <t>El sistema debe optimizar las imágenes para carga rápida.</t>
   </si>
   <si>
     <t>El sistema debe mantener el carrito de compras entre sesiones del usuario.</t>
-  </si>
-  <si>
-    <t>El sistema debe mostrar animaciones suaves en las transiciones visuales.</t>
   </si>
   <si>
     <t>El sistema debe cerrar automáticamente los menús desplegables al hacer clic fuera de ellos.</t>
@@ -1300,50 +1294,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1361,6 +1314,50 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1371,20 +1368,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1688,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:I66"/>
+  <dimension ref="B2:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView topLeftCell="C36" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,16 +1699,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="47" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="B2" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1749,20 +1743,20 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="28"/>
       <c r="F9" s="3" t="s">
         <v>0</v>
       </c>
@@ -1782,7 +1776,7 @@
         <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1796,7 +1790,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1810,7 +1804,7 @@
         <v>55</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1824,7 +1818,7 @@
         <v>56</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1838,7 +1832,7 @@
         <v>57</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1849,10 +1843,10 @@
         <v>6</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1866,7 +1860,7 @@
         <v>58</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1880,7 +1874,7 @@
         <v>59</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1894,7 +1888,7 @@
         <v>60</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1908,7 +1902,7 @@
         <v>61</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1922,7 +1916,7 @@
         <v>62</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1936,7 +1930,7 @@
         <v>63</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1950,7 +1944,7 @@
         <v>64</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1964,7 +1958,7 @@
         <v>65</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1978,7 +1972,7 @@
         <v>66</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1992,7 +1986,7 @@
         <v>67</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2006,7 +2000,7 @@
         <v>68</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -2020,7 +2014,7 @@
         <v>69</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -2034,7 +2028,7 @@
         <v>70</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -2045,10 +2039,10 @@
         <v>20</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -2056,13 +2050,13 @@
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>71</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -2070,13 +2064,13 @@
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="5">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>72</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -2084,13 +2078,13 @@
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>73</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2098,13 +2092,13 @@
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="5">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>74</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2112,13 +2106,13 @@
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="5">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>75</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2126,13 +2120,13 @@
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="5">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>76</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2140,13 +2134,13 @@
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="5">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>77</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2154,13 +2148,13 @@
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="5">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>78</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2168,13 +2162,13 @@
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="5">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>79</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -2182,13 +2176,13 @@
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="5">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>80</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -2196,13 +2190,13 @@
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="5">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -2210,13 +2204,13 @@
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="5">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>81</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -2224,27 +2218,27 @@
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="5">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>82</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="5">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>83</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2252,13 +2246,13 @@
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="5">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>84</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2266,13 +2260,13 @@
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="5">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>85</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -2280,13 +2274,13 @@
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="5">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>86</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2294,23 +2288,23 @@
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" s="5">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>87</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="50"/>
+      <c r="D49" s="29"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F50" s="7" t="s">
@@ -2334,7 +2328,7 @@
         <v>88</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -2348,11 +2342,9 @@
         <v>89</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>291</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
@@ -2364,7 +2356,7 @@
         <v>90</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -2378,7 +2370,7 @@
         <v>91</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -2391,7 +2383,9 @@
       <c r="D55" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F55" s="2"/>
+      <c r="F55" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -2401,10 +2395,10 @@
         <v>6</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -2415,10 +2409,10 @@
         <v>7</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -2432,7 +2426,7 @@
         <v>94</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -2443,10 +2437,10 @@
         <v>9</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>95</v>
+        <v>297</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -2457,76 +2451,74 @@
         <v>10</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>96</v>
+        <v>298</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
     <row r="61" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C61" s="58">
+      <c r="C61" s="5">
         <v>11</v>
       </c>
-      <c r="D61" s="59" t="s">
+      <c r="D61" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="F61" s="60" t="s">
-        <v>291</v>
-      </c>
+      <c r="F61" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="58">
+      <c r="C62" s="5">
         <v>12</v>
       </c>
-      <c r="D62" s="59" t="s">
+      <c r="D62" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="F62" s="60" t="s">
-        <v>291</v>
-      </c>
+      <c r="F62" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="58">
+      <c r="C63" s="5">
         <v>13</v>
       </c>
-      <c r="D63" s="59" t="s">
+      <c r="D63" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="F63" s="60" t="s">
-        <v>291</v>
-      </c>
+      <c r="F63" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C64" s="58">
+      <c r="C64" s="5">
         <v>14</v>
       </c>
-      <c r="D64" s="59" t="s">
+      <c r="D64" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="F64" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C65" s="58">
-        <v>15</v>
-      </c>
-      <c r="D65" s="59" t="s">
-        <v>303</v>
-      </c>
-      <c r="F65" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C66" s="58">
-        <v>16</v>
-      </c>
-      <c r="D66" s="59" t="s">
-        <v>304</v>
+      <c r="F64" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="58">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2560,25 +2552,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -2589,10 +2581,10 @@
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="42"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -2603,10 +2595,10 @@
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -2614,10 +2606,10 @@
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="12" t="s">
         <v>7</v>
       </c>
@@ -2627,11 +2619,11 @@
       <c r="I6" s="13"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
       <c r="F9" s="20" t="s">
         <v>0</v>
       </c>
@@ -2649,10 +2641,10 @@
       <c r="B10" s="15">
         <v>1</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="D10" s="38"/>
+      <c r="C10" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" s="39"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2663,7 +2655,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D11" s="31"/>
       <c r="F11" s="2"/>
@@ -2689,7 +2681,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D13" s="31"/>
       <c r="F13" s="2"/>
@@ -2702,7 +2694,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D14" s="31"/>
       <c r="F14" s="2"/>
@@ -2715,7 +2707,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D15" s="31"/>
       <c r="F15" s="2"/>
@@ -2727,10 +2719,10 @@
       <c r="B16" s="16">
         <v>7</v>
       </c>
-      <c r="C16" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="D16" s="25"/>
+      <c r="C16" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="D16" s="41"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -2754,7 +2746,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D18" s="31"/>
       <c r="F18" s="2"/>
@@ -2767,7 +2759,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D19" s="31"/>
       <c r="F19" s="2"/>
@@ -2793,7 +2785,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D21" s="31"/>
       <c r="F21" s="2"/>
@@ -2806,7 +2798,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D22" s="31"/>
       <c r="F22" s="2"/>
@@ -2819,7 +2811,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D23" s="31"/>
       <c r="F23" s="2"/>
@@ -2832,7 +2824,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D24" s="31"/>
       <c r="F24" s="2"/>
@@ -2844,8 +2836,8 @@
       <c r="B25" s="16">
         <v>16</v>
       </c>
-      <c r="C25" s="36" t="s">
-        <v>222</v>
+      <c r="C25" s="42" t="s">
+        <v>220</v>
       </c>
       <c r="D25" s="31"/>
       <c r="F25" s="2"/>
@@ -2858,7 +2850,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D26" s="31"/>
       <c r="F26" s="2"/>
@@ -2871,7 +2863,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D27" s="31"/>
       <c r="F27" s="2"/>
@@ -2884,7 +2876,7 @@
         <v>19</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D28" s="31"/>
       <c r="F28" s="2"/>
@@ -2897,7 +2889,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D29" s="31"/>
       <c r="F29" s="2"/>
@@ -2909,29 +2901,29 @@
       <c r="B30" s="16">
         <v>21</v>
       </c>
-      <c r="C30" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="D30" s="33"/>
+      <c r="C30" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="D30" s="45"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
       <c r="F33" s="20" t="s">
         <v>0</v>
       </c>
@@ -2949,10 +2941,10 @@
       <c r="B34" s="17">
         <v>1</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="D34" s="25"/>
+      <c r="C34" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="D34" s="41"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2962,10 +2954,10 @@
       <c r="B35" s="18">
         <v>2</v>
       </c>
-      <c r="C35" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="D35" s="25"/>
+      <c r="C35" s="43" t="s">
+        <v>227</v>
+      </c>
+      <c r="D35" s="41"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2975,10 +2967,10 @@
       <c r="B36" s="18">
         <v>3</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="D36" s="25"/>
+      <c r="C36" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="D36" s="41"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2988,10 +2980,10 @@
       <c r="B37" s="18">
         <v>4</v>
       </c>
-      <c r="C37" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="D37" s="25"/>
+      <c r="C37" s="43" t="s">
+        <v>229</v>
+      </c>
+      <c r="D37" s="41"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -3001,10 +2993,10 @@
       <c r="B38" s="18">
         <v>5</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="D38" s="25"/>
+      <c r="C38" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="D38" s="41"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -3014,10 +3006,10 @@
       <c r="B39" s="18">
         <v>7</v>
       </c>
-      <c r="C39" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="D39" s="25"/>
+      <c r="C39" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="D39" s="41"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -3027,10 +3019,10 @@
       <c r="B40" s="18">
         <v>8</v>
       </c>
-      <c r="C40" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="D40" s="25"/>
+      <c r="C40" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="D40" s="41"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -3040,10 +3032,10 @@
       <c r="B41" s="18">
         <v>9</v>
       </c>
-      <c r="C41" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="D41" s="25"/>
+      <c r="C41" s="40" t="s">
+        <v>233</v>
+      </c>
+      <c r="D41" s="41"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -3053,10 +3045,10 @@
       <c r="B42" s="18">
         <v>10</v>
       </c>
-      <c r="C42" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="D42" s="25"/>
+      <c r="C42" s="40" t="s">
+        <v>234</v>
+      </c>
+      <c r="D42" s="41"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -3066,10 +3058,10 @@
       <c r="B43" s="18">
         <v>11</v>
       </c>
-      <c r="C43" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="D43" s="25"/>
+      <c r="C43" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D43" s="41"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -3079,10 +3071,10 @@
       <c r="B44" s="18">
         <v>12</v>
       </c>
-      <c r="C44" s="24" t="s">
-        <v>238</v>
-      </c>
-      <c r="D44" s="25"/>
+      <c r="C44" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="D44" s="41"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -3092,10 +3084,10 @@
       <c r="B45" s="18">
         <v>13</v>
       </c>
-      <c r="C45" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="D45" s="25"/>
+      <c r="C45" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D45" s="41"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -3105,10 +3097,10 @@
       <c r="B46" s="18">
         <v>14</v>
       </c>
-      <c r="C46" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="D46" s="29"/>
+      <c r="C46" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="D46" s="48"/>
       <c r="E46" s="14"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -3119,10 +3111,10 @@
       <c r="B47" s="19">
         <v>15</v>
       </c>
-      <c r="C47" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="D47" s="25"/>
+      <c r="C47" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="41"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -3132,10 +3124,10 @@
       <c r="B48" s="18">
         <v>16</v>
       </c>
-      <c r="C48" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="D48" s="25"/>
+      <c r="C48" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="D48" s="41"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -3145,10 +3137,10 @@
       <c r="B49" s="18">
         <v>17</v>
       </c>
-      <c r="C49" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="D49" s="25"/>
+      <c r="C49" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="D49" s="41"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -3158,10 +3150,10 @@
       <c r="B50" s="18">
         <v>18</v>
       </c>
-      <c r="C50" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D50" s="25"/>
+      <c r="C50" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="D50" s="41"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -3171,10 +3163,10 @@
       <c r="B51" s="18">
         <v>19</v>
       </c>
-      <c r="C51" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="D51" s="25"/>
+      <c r="C51" s="40" t="s">
+        <v>242</v>
+      </c>
+      <c r="D51" s="41"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3184,10 +3176,10 @@
       <c r="B52" s="18">
         <v>20</v>
       </c>
-      <c r="C52" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="D52" s="25"/>
+      <c r="C52" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="D52" s="41"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -3197,10 +3189,10 @@
       <c r="B53" s="18">
         <v>21</v>
       </c>
-      <c r="C53" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="D53" s="25"/>
+      <c r="C53" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="D53" s="41"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3210,85 +3202,141 @@
       <c r="B54" s="18">
         <v>22</v>
       </c>
-      <c r="C54" s="26" t="s">
-        <v>247</v>
-      </c>
-      <c r="D54" s="27"/>
+      <c r="C54" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="D54" s="51"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="49"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="49"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="49"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="49"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="49"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="49"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="23"/>
-      <c r="D77" s="23"/>
+      <c r="C77" s="49"/>
+      <c r="D77" s="49"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="23"/>
-      <c r="D78" s="23"/>
+      <c r="C78" s="49"/>
+      <c r="D78" s="49"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
+      <c r="C79" s="49"/>
+      <c r="D79" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="C3:D3"/>
@@ -3301,62 +3349,6 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3384,16 +3376,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="47" t="s">
-        <v>205</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="B2" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -3428,20 +3420,20 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="28"/>
       <c r="F9" s="3" t="s">
         <v>0</v>
       </c>
@@ -3826,10 +3818,10 @@
       <c r="I40" s="2"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="51" t="s">
+      <c r="C42" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="51"/>
+      <c r="D42" s="52"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F43" s="3" t="s">
@@ -3959,16 +3951,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="B2" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -4003,20 +3995,20 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="52"/>
       <c r="F9" s="3" t="s">
         <v>0</v>
       </c>
@@ -4033,7 +4025,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -4045,7 +4037,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -4057,7 +4049,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -4069,7 +4061,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -4081,7 +4073,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -4093,7 +4085,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -4105,7 +4097,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -4117,7 +4109,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4129,7 +4121,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -4141,7 +4133,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -4153,7 +4145,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -4165,7 +4157,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -4177,7 +4169,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -4189,7 +4181,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -4201,7 +4193,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -4213,7 +4205,7 @@
         <v>16</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -4225,7 +4217,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -4237,7 +4229,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -4249,7 +4241,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -4261,7 +4253,7 @@
         <v>20</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -4273,7 +4265,7 @@
         <v>21</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -4285,7 +4277,7 @@
         <v>22</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -4297,7 +4289,7 @@
         <v>23</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -4309,7 +4301,7 @@
         <v>24</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -4321,7 +4313,7 @@
         <v>25</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -4333,7 +4325,7 @@
         <v>26</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -4345,7 +4337,7 @@
         <v>27</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -4357,7 +4349,7 @@
         <v>28</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -4369,7 +4361,7 @@
         <v>29</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -4381,7 +4373,7 @@
         <v>30</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -4393,7 +4385,7 @@
         <v>31</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -4405,7 +4397,7 @@
         <v>32</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -4417,7 +4409,7 @@
         <v>33</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -4429,7 +4421,7 @@
         <v>34</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -4441,7 +4433,7 @@
         <v>35</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -4449,10 +4441,10 @@
       <c r="I44" s="2"/>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="51" t="s">
+      <c r="C46" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="51"/>
+      <c r="D46" s="52"/>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F47" s="3" t="s">
@@ -4473,7 +4465,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -4485,7 +4477,7 @@
         <v>2</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -4497,7 +4489,7 @@
         <v>3</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -4509,7 +4501,7 @@
         <v>4</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -4521,7 +4513,7 @@
         <v>5</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -4533,7 +4525,7 @@
         <v>6</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -4545,7 +4537,7 @@
         <v>7</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -4557,7 +4549,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -4606,16 +4598,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="B2" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -4650,20 +4642,20 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
       <c r="I8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="52"/>
       <c r="F9" s="3" t="s">
         <v>0</v>
       </c>
@@ -4680,7 +4672,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -4692,7 +4684,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -4704,7 +4696,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -4716,7 +4708,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -4728,7 +4720,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -4740,7 +4732,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -4752,7 +4744,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -4764,7 +4756,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4776,7 +4768,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -4788,7 +4780,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -4800,7 +4792,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -4812,7 +4804,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -4824,7 +4816,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -4836,7 +4828,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -4848,7 +4840,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -4860,7 +4852,7 @@
         <v>16</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -4872,7 +4864,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -4884,7 +4876,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -4896,7 +4888,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -4908,7 +4900,7 @@
         <v>20</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -4920,7 +4912,7 @@
         <v>21</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -4932,7 +4924,7 @@
         <v>22</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -4944,7 +4936,7 @@
         <v>23</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -4956,7 +4948,7 @@
         <v>24</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -4968,7 +4960,7 @@
         <v>25</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -4980,7 +4972,7 @@
         <v>26</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -4992,7 +4984,7 @@
         <v>27</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -5004,7 +4996,7 @@
         <v>28</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -5016,7 +5008,7 @@
         <v>29</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -5028,7 +5020,7 @@
         <v>30</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -5040,7 +5032,7 @@
         <v>31</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -5052,7 +5044,7 @@
         <v>32</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -5064,7 +5056,7 @@
         <v>33</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -5076,7 +5068,7 @@
         <v>34</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -5088,7 +5080,7 @@
         <v>35</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -5100,7 +5092,7 @@
         <v>36</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -5112,7 +5104,7 @@
         <v>37</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -5124,7 +5116,7 @@
         <v>38</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -5136,7 +5128,7 @@
         <v>39</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -5148,7 +5140,7 @@
         <v>40</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -5160,7 +5152,7 @@
         <v>41</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -5172,7 +5164,7 @@
         <v>42</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -5184,7 +5176,7 @@
         <v>43</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -5196,7 +5188,7 @@
         <v>44</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -5204,10 +5196,10 @@
       <c r="I53" s="2"/>
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="51" t="s">
+      <c r="C55" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="51"/>
+      <c r="D55" s="52"/>
     </row>
     <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F56" s="3" t="s">
@@ -5228,7 +5220,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -5240,7 +5232,7 @@
         <v>2</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -5252,7 +5244,7 @@
         <v>3</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -5264,7 +5256,7 @@
         <v>4</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -5276,7 +5268,7 @@
         <v>5</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -5288,7 +5280,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -5300,7 +5292,7 @@
         <v>7</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -5312,7 +5304,7 @@
         <v>8</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -5336,7 +5328,7 @@
         <v>10</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -5374,16 +5366,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="B2" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -5418,20 +5410,20 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
       <c r="I8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="52"/>
       <c r="F9" s="3" t="s">
         <v>0</v>
       </c>
@@ -5448,7 +5440,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -5460,7 +5452,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -5472,7 +5464,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -5484,7 +5476,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -5496,7 +5488,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -5508,7 +5500,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -5520,7 +5512,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -5532,7 +5524,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5544,7 +5536,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -5556,7 +5548,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -5568,7 +5560,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -5576,10 +5568,10 @@
       <c r="I20" s="2"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="51"/>
+      <c r="D22" s="52"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F23" s="3" t="s">
@@ -5600,7 +5592,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -5612,7 +5604,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -5624,7 +5616,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -5648,7 +5640,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -5670,8 +5662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F66246-78FA-4E46-BC75-E6EFAC710DAD}">
   <dimension ref="B2:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="B36" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5683,25 +5675,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
-        <v>248</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -5712,10 +5704,10 @@
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="42"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -5726,10 +5718,10 @@
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -5737,10 +5729,10 @@
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="12" t="s">
         <v>7</v>
       </c>
@@ -5750,11 +5742,11 @@
       <c r="I6" s="13"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
       <c r="F9" s="20" t="s">
         <v>0</v>
       </c>
@@ -5773,11 +5765,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D10" s="56"/>
-      <c r="F10" s="57" t="s">
-        <v>291</v>
+      <c r="F10" s="22" t="s">
+        <v>289</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -5788,11 +5780,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D11" s="56"/>
-      <c r="F11" s="57" t="s">
-        <v>291</v>
+      <c r="F11" s="22" t="s">
+        <v>289</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -5803,11 +5795,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D12" s="56"/>
       <c r="F12" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -5818,11 +5810,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D13" s="56"/>
       <c r="F13" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -5833,11 +5825,11 @@
         <v>5</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D14" s="56"/>
       <c r="F14" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -5848,11 +5840,11 @@
         <v>7</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D15" s="56"/>
       <c r="F15" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -5863,11 +5855,11 @@
         <v>8</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D16" s="56"/>
       <c r="F16" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -5878,11 +5870,11 @@
         <v>9</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D17" s="56"/>
       <c r="F17" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -5893,14 +5885,14 @@
         <v>11</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D18" s="56"/>
       <c r="F18" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -5910,14 +5902,14 @@
         <v>12</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D19" s="56"/>
       <c r="F19" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -5927,14 +5919,14 @@
         <v>13</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D20" s="56"/>
       <c r="F20" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -5944,14 +5936,14 @@
         <v>14</v>
       </c>
       <c r="C21" s="56" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D21" s="56"/>
       <c r="F21" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -5961,11 +5953,11 @@
         <v>15</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D22" s="56"/>
       <c r="F22" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -5976,11 +5968,11 @@
         <v>16</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D23" s="56"/>
       <c r="F23" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -5991,11 +5983,11 @@
         <v>17</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D24" s="56"/>
       <c r="F24" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -6006,11 +5998,11 @@
         <v>18</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D25" s="56"/>
       <c r="F25" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -6021,15 +6013,13 @@
         <v>19</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D26" s="56"/>
       <c r="F26" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>291</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
@@ -6038,11 +6028,11 @@
         <v>20</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D27" s="56"/>
       <c r="F27" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -6053,15 +6043,13 @@
         <v>21</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D28" s="56"/>
       <c r="F28" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>291</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
@@ -6070,15 +6058,13 @@
         <v>22</v>
       </c>
       <c r="C29" s="56" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D29" s="56"/>
       <c r="F29" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>291</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
@@ -6086,16 +6072,14 @@
       <c r="B30" s="16">
         <v>24</v>
       </c>
-      <c r="C30" s="55" t="s">
-        <v>268</v>
-      </c>
-      <c r="D30" s="55"/>
+      <c r="C30" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="D30" s="57"/>
       <c r="F30" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>291</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
@@ -6104,15 +6088,13 @@
         <v>25</v>
       </c>
       <c r="C31" s="56" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D31" s="56"/>
       <c r="F31" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>291</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
@@ -6120,12 +6102,12 @@
       <c r="B32" s="16">
         <v>26</v>
       </c>
-      <c r="C32" s="55" t="s">
-        <v>270</v>
-      </c>
-      <c r="D32" s="55"/>
+      <c r="C32" s="57" t="s">
+        <v>268</v>
+      </c>
+      <c r="D32" s="57"/>
       <c r="F32" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -6135,12 +6117,12 @@
       <c r="B33" s="16">
         <v>30</v>
       </c>
-      <c r="C33" s="55" t="s">
-        <v>271</v>
-      </c>
-      <c r="D33" s="55"/>
+      <c r="C33" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="D33" s="57"/>
       <c r="F33" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -6150,12 +6132,12 @@
       <c r="B34" s="16">
         <v>31</v>
       </c>
-      <c r="C34" s="55" t="s">
-        <v>272</v>
-      </c>
-      <c r="D34" s="55"/>
+      <c r="C34" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="D34" s="57"/>
       <c r="F34" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -6165,12 +6147,12 @@
       <c r="B35" s="16">
         <v>32</v>
       </c>
-      <c r="C35" s="55" t="s">
-        <v>273</v>
-      </c>
-      <c r="D35" s="55"/>
+      <c r="C35" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="57"/>
       <c r="F35" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -6180,12 +6162,12 @@
       <c r="B36" s="16">
         <v>33</v>
       </c>
-      <c r="C36" s="55" t="s">
-        <v>274</v>
-      </c>
-      <c r="D36" s="55"/>
+      <c r="C36" s="57" t="s">
+        <v>272</v>
+      </c>
+      <c r="D36" s="57"/>
       <c r="F36" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -6195,12 +6177,12 @@
       <c r="B37" s="16">
         <v>34</v>
       </c>
-      <c r="C37" s="55" t="s">
-        <v>293</v>
-      </c>
-      <c r="D37" s="55"/>
+      <c r="C37" s="57" t="s">
+        <v>291</v>
+      </c>
+      <c r="D37" s="57"/>
       <c r="F37" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -6210,12 +6192,12 @@
       <c r="B38" s="16">
         <v>35</v>
       </c>
-      <c r="C38" s="55" t="s">
-        <v>275</v>
-      </c>
-      <c r="D38" s="55"/>
+      <c r="C38" s="57" t="s">
+        <v>273</v>
+      </c>
+      <c r="D38" s="57"/>
       <c r="F38" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -6225,13 +6207,13 @@
       <c r="B39" s="16">
         <v>36</v>
       </c>
-      <c r="C39" s="55" t="s">
-        <v>276</v>
-      </c>
-      <c r="D39" s="55"/>
+      <c r="C39" s="57" t="s">
+        <v>274</v>
+      </c>
+      <c r="D39" s="57"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -6240,12 +6222,12 @@
       <c r="B40" s="16">
         <v>38</v>
       </c>
-      <c r="C40" s="55" t="s">
-        <v>277</v>
-      </c>
-      <c r="D40" s="55"/>
+      <c r="C40" s="57" t="s">
+        <v>275</v>
+      </c>
+      <c r="D40" s="57"/>
       <c r="F40" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -6255,12 +6237,12 @@
       <c r="B41" s="16">
         <v>39</v>
       </c>
-      <c r="C41" s="55" t="s">
-        <v>294</v>
-      </c>
-      <c r="D41" s="55"/>
+      <c r="C41" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="D41" s="57"/>
       <c r="F41" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -6270,12 +6252,12 @@
       <c r="B42" s="16">
         <v>40</v>
       </c>
-      <c r="C42" s="55" t="s">
-        <v>278</v>
-      </c>
-      <c r="D42" s="55"/>
+      <c r="C42" s="57" t="s">
+        <v>276</v>
+      </c>
+      <c r="D42" s="57"/>
       <c r="F42" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -6285,12 +6267,12 @@
       <c r="B43" s="16">
         <v>41</v>
       </c>
-      <c r="C43" s="55" t="s">
-        <v>279</v>
-      </c>
-      <c r="D43" s="55"/>
+      <c r="C43" s="57" t="s">
+        <v>277</v>
+      </c>
+      <c r="D43" s="57"/>
       <c r="F43" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -6300,12 +6282,12 @@
       <c r="B44" s="16">
         <v>42</v>
       </c>
-      <c r="C44" s="55" t="s">
-        <v>280</v>
-      </c>
-      <c r="D44" s="55"/>
+      <c r="C44" s="57" t="s">
+        <v>278</v>
+      </c>
+      <c r="D44" s="57"/>
       <c r="F44" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -6315,12 +6297,12 @@
       <c r="B45" s="16">
         <v>43</v>
       </c>
-      <c r="C45" s="55" t="s">
-        <v>281</v>
-      </c>
-      <c r="D45" s="55"/>
+      <c r="C45" s="57" t="s">
+        <v>279</v>
+      </c>
+      <c r="D45" s="57"/>
       <c r="F45" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -6330,12 +6312,12 @@
       <c r="B46" s="16">
         <v>44</v>
       </c>
-      <c r="C46" s="55" t="s">
-        <v>282</v>
-      </c>
-      <c r="D46" s="55"/>
+      <c r="C46" s="57" t="s">
+        <v>280</v>
+      </c>
+      <c r="D46" s="57"/>
       <c r="F46" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -6345,12 +6327,12 @@
       <c r="B47" s="16">
         <v>45</v>
       </c>
-      <c r="C47" s="55" t="s">
-        <v>283</v>
-      </c>
-      <c r="D47" s="55"/>
+      <c r="C47" s="57" t="s">
+        <v>281</v>
+      </c>
+      <c r="D47" s="57"/>
       <c r="F47" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -6360,12 +6342,12 @@
       <c r="B48" s="16">
         <v>46</v>
       </c>
-      <c r="C48" s="55" t="s">
-        <v>295</v>
-      </c>
-      <c r="D48" s="55"/>
+      <c r="C48" s="57" t="s">
+        <v>293</v>
+      </c>
+      <c r="D48" s="57"/>
       <c r="F48" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -6375,13 +6357,13 @@
       <c r="B49" s="16">
         <v>47</v>
       </c>
-      <c r="C49" s="55" t="s">
-        <v>284</v>
-      </c>
-      <c r="D49" s="55"/>
+      <c r="C49" s="57" t="s">
+        <v>282</v>
+      </c>
+      <c r="D49" s="57"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -6390,12 +6372,12 @@
       <c r="B50" s="16">
         <v>48</v>
       </c>
-      <c r="C50" s="55" t="s">
-        <v>285</v>
-      </c>
-      <c r="D50" s="55"/>
+      <c r="C50" s="57" t="s">
+        <v>283</v>
+      </c>
+      <c r="D50" s="57"/>
       <c r="F50" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -6405,12 +6387,12 @@
       <c r="B51" s="16">
         <v>50</v>
       </c>
-      <c r="C51" s="55" t="s">
-        <v>286</v>
-      </c>
-      <c r="D51" s="55"/>
+      <c r="C51" s="57" t="s">
+        <v>284</v>
+      </c>
+      <c r="D51" s="57"/>
       <c r="F51" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -6420,12 +6402,12 @@
       <c r="B52" s="16">
         <v>51</v>
       </c>
-      <c r="C52" s="55" t="s">
-        <v>287</v>
-      </c>
-      <c r="D52" s="55"/>
+      <c r="C52" s="57" t="s">
+        <v>285</v>
+      </c>
+      <c r="D52" s="57"/>
       <c r="F52" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -6435,12 +6417,12 @@
       <c r="B53" s="16">
         <v>52</v>
       </c>
-      <c r="C53" s="55" t="s">
-        <v>288</v>
-      </c>
-      <c r="D53" s="55"/>
+      <c r="C53" s="57" t="s">
+        <v>286</v>
+      </c>
+      <c r="D53" s="57"/>
       <c r="F53" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -6450,15 +6432,13 @@
       <c r="B54" s="16">
         <v>53</v>
       </c>
-      <c r="C54" s="55" t="s">
-        <v>289</v>
-      </c>
-      <c r="D54" s="55"/>
-      <c r="F54" s="2" t="s">
-        <v>291</v>
-      </c>
+      <c r="C54" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="D54" s="57"/>
+      <c r="F54" s="2"/>
       <c r="G54" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -6467,61 +6447,97 @@
       <c r="B55" s="16">
         <v>54</v>
       </c>
-      <c r="C55" s="55" t="s">
-        <v>290</v>
-      </c>
-      <c r="D55" s="55"/>
+      <c r="C55" s="57" t="s">
+        <v>288</v>
+      </c>
+      <c r="D55" s="57"/>
       <c r="F55" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="24"/>
-      <c r="D56" s="22"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="24"/>
-      <c r="D57" s="22"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="24"/>
-      <c r="D58" s="22"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="60"/>
+      <c r="D58" s="60"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="24"/>
-      <c r="D59" s="22"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="60"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C60" s="24"/>
-      <c r="D60" s="22"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="60"/>
+      <c r="D60" s="60"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C61" s="24"/>
-      <c r="D61" s="22"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="24"/>
-      <c r="D62" s="22"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="60"/>
+      <c r="D62" s="60"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="24"/>
-      <c r="D63" s="22"/>
+      <c r="B63" s="59"/>
+      <c r="C63" s="60"/>
+      <c r="D63" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C15:D15"/>
@@ -6534,44 +6550,16 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>